<commit_message>
fix typos assignment 2
</commit_message>
<xml_diff>
--- a/assignments/Assignment 02/Solución Tarea 2 .xlsx
+++ b/assignments/Assignment 02/Solución Tarea 2 .xlsx
@@ -5,21 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cinthyaandrade/Desktop/class_ITAM_estadistica1/Soluciones Tareas /"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salvadorgarcia/Repos/class_ITAM_estadistica1/assignments/Assignment 02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA84EEC-0F8E-8548-847D-B201BA946689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D80352-9DFD-754B-A398-14C2AB9DB5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{635F2F8D-BD2C-0949-864D-D988A36D99BE}"/>
+    <workbookView xWindow="22220" yWindow="1400" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{635F2F8D-BD2C-0949-864D-D988A36D99BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Pregunta 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Pregunta 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
   <si>
     <t xml:space="preserve">DATOS </t>
   </si>
@@ -60,9 +57,6 @@
   </si>
   <si>
     <t xml:space="preserve">3. amplitud de clase </t>
-  </si>
-  <si>
-    <t xml:space="preserve">diferencia </t>
   </si>
   <si>
     <t xml:space="preserve">CLASES </t>
@@ -259,11 +253,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0000000000"/>
-    <numFmt numFmtId="165" formatCode="0.000%"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -459,20 +453,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -483,30 +471,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -528,12 +507,27 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares 2" xfId="3" xr:uid="{587E1681-1867-3E4B-BEDA-D41016B85A9D}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{E5F3800B-1327-5C48-BF43-372C5714F6FF}"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Porcentaje 2" xfId="4" xr:uid="{E6AAD82F-9669-0847-AAB6-E084498E3DEC}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,7 +546,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -589,7 +583,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="en-MX"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -635,16 +629,16 @@
                   <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3519999999999999</c:v>
+                  <c:v>2.3420000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4539999999999997</c:v>
+                  <c:v>2.4340000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5559999999999996</c:v>
+                  <c:v>2.5260000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6579999999999995</c:v>
+                  <c:v>2.6180000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -733,7 +727,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="en-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1657482095"/>
@@ -792,7 +786,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="en-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1651270431"/>
@@ -833,7 +827,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="en-MX"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -847,7 +841,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -884,7 +878,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="en-MX"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -930,16 +924,16 @@
                   <c:v>2.3420000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.444</c:v>
+                  <c:v>2.4340000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5459999999999998</c:v>
+                  <c:v>2.5260000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6479999999999997</c:v>
+                  <c:v>2.6180000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7499999999999996</c:v>
+                  <c:v>2.7100000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1028,7 +1022,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="en-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1657186351"/>
@@ -1087,7 +1081,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="en-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1471714959"/>
@@ -1128,7 +1122,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="en-MX"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1142,7 +1136,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1204,7 +1198,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="en-MX"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1249,16 +1243,16 @@
                   <c:v>2.2960000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3979999999999997</c:v>
+                  <c:v>2.3879999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5</c:v>
+                  <c:v>2.4800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6019999999999994</c:v>
+                  <c:v>2.5720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7039999999999997</c:v>
+                  <c:v>2.6640000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1347,7 +1341,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="en-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1921232527"/>
@@ -1406,7 +1400,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="en-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1650651039"/>
@@ -1447,7 +1441,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="en-MX"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1461,7 +1455,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1528,7 +1522,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="en-MX"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1573,16 +1567,16 @@
                   <c:v>2.2960000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3979999999999997</c:v>
+                  <c:v>2.3879999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5</c:v>
+                  <c:v>2.4800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6019999999999994</c:v>
+                  <c:v>2.5720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7039999999999997</c:v>
+                  <c:v>2.6640000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1669,16 +1663,16 @@
                   <c:v>2.2960000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3979999999999997</c:v>
+                  <c:v>2.3879999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5</c:v>
+                  <c:v>2.4800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6019999999999994</c:v>
+                  <c:v>2.5720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7039999999999997</c:v>
+                  <c:v>2.6640000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1768,7 +1762,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="en-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1546156255"/>
@@ -1827,7 +1821,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="en-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1650869263"/>
@@ -1869,7 +1863,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="en-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="998947456"/>
@@ -1928,7 +1922,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="en-MX"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1942,7 +1936,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-MX"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2004,7 +1998,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-MX"/>
+          <a:endParaRPr lang="en-MX"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2221,7 +2215,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="en-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2052993375"/>
@@ -2283,7 +2277,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-MX"/>
+            <a:endParaRPr lang="en-MX"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1921829871"/>
@@ -2324,7 +2318,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-MX"/>
+      <a:endParaRPr lang="en-MX"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5438,492 +5432,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Pregunta 1"/>
-      <sheetName val="Calculos de la preg 2 "/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="7">
-          <cell r="L7">
-            <v>1</v>
-          </cell>
-          <cell r="M7">
-            <v>2.15</v>
-          </cell>
-          <cell r="O7">
-            <v>2.25</v>
-          </cell>
-          <cell r="P7">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="L8">
-            <v>1</v>
-          </cell>
-          <cell r="M8">
-            <v>2.1800000000000002</v>
-          </cell>
-          <cell r="O8">
-            <v>2.27</v>
-          </cell>
-          <cell r="P8">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="L9">
-            <v>1</v>
-          </cell>
-          <cell r="M9">
-            <v>2.19</v>
-          </cell>
-          <cell r="O9">
-            <v>2.27</v>
-          </cell>
-          <cell r="P9">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="L10">
-            <v>2</v>
-          </cell>
-          <cell r="M10">
-            <v>2.19</v>
-          </cell>
-          <cell r="O10">
-            <v>2.27</v>
-          </cell>
-          <cell r="P10">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="L11">
-            <v>3</v>
-          </cell>
-          <cell r="M11">
-            <v>2.19</v>
-          </cell>
-          <cell r="O11">
-            <v>2.27</v>
-          </cell>
-          <cell r="P11">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="L12">
-            <v>4</v>
-          </cell>
-          <cell r="M12">
-            <v>2.19</v>
-          </cell>
-          <cell r="O12">
-            <v>2.27</v>
-          </cell>
-          <cell r="P12">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="L13">
-            <v>1</v>
-          </cell>
-          <cell r="M13">
-            <v>2.21</v>
-          </cell>
-          <cell r="O13">
-            <v>2.27</v>
-          </cell>
-          <cell r="P13">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="L14">
-            <v>1</v>
-          </cell>
-          <cell r="M14">
-            <v>2.27</v>
-          </cell>
-          <cell r="O14">
-            <v>2.27</v>
-          </cell>
-          <cell r="P14">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="L15">
-            <v>2</v>
-          </cell>
-          <cell r="M15">
-            <v>2.27</v>
-          </cell>
-          <cell r="O15">
-            <v>2.36</v>
-          </cell>
-          <cell r="P15">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="L16">
-            <v>3</v>
-          </cell>
-          <cell r="M16">
-            <v>2.27</v>
-          </cell>
-          <cell r="O16">
-            <v>2.4</v>
-          </cell>
-          <cell r="P16">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="L17">
-            <v>4</v>
-          </cell>
-          <cell r="M17">
-            <v>2.27</v>
-          </cell>
-          <cell r="O17">
-            <v>2.4</v>
-          </cell>
-          <cell r="P17">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="L18">
-            <v>5</v>
-          </cell>
-          <cell r="M18">
-            <v>2.27</v>
-          </cell>
-          <cell r="O18">
-            <v>2.4900000000000002</v>
-          </cell>
-          <cell r="P18">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="L19">
-            <v>6</v>
-          </cell>
-          <cell r="M19">
-            <v>2.27</v>
-          </cell>
-          <cell r="O19">
-            <v>2.5</v>
-          </cell>
-          <cell r="P19">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="L20">
-            <v>1</v>
-          </cell>
-          <cell r="M20">
-            <v>2.2999999999999998</v>
-          </cell>
-          <cell r="O20">
-            <v>2.56</v>
-          </cell>
-          <cell r="P20">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="L21">
-            <v>1</v>
-          </cell>
-          <cell r="M21">
-            <v>2.33</v>
-          </cell>
-          <cell r="O21">
-            <v>2.71</v>
-          </cell>
-          <cell r="P21">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="F34" t="str">
-            <v xml:space="preserve">Frecuencia Absoluta </v>
-          </cell>
-          <cell r="G34" t="str">
-            <v xml:space="preserve">Frecuencia Relativa </v>
-          </cell>
-          <cell r="M34" t="str">
-            <v xml:space="preserve">Mayor que </v>
-          </cell>
-          <cell r="N34" t="str">
-            <v xml:space="preserve">Menor que </v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>2.15</v>
-          </cell>
-          <cell r="D35">
-            <v>2.1859999999999999</v>
-          </cell>
-          <cell r="E35">
-            <v>2.1680000000000001</v>
-          </cell>
-          <cell r="F35">
-            <v>2</v>
-          </cell>
-          <cell r="G35">
-            <v>0.13333333333333333</v>
-          </cell>
-          <cell r="M35">
-            <v>15</v>
-          </cell>
-          <cell r="N35">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36">
-            <v>2.1959999999999997</v>
-          </cell>
-          <cell r="D36">
-            <v>2.2319999999999998</v>
-          </cell>
-          <cell r="E36">
-            <v>2.2139999999999995</v>
-          </cell>
-          <cell r="F36">
-            <v>5</v>
-          </cell>
-          <cell r="G36">
-            <v>0.33333333333333331</v>
-          </cell>
-          <cell r="M36">
-            <v>13</v>
-          </cell>
-          <cell r="N36">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37">
-            <v>2.2419999999999995</v>
-          </cell>
-          <cell r="D37">
-            <v>2.2779999999999996</v>
-          </cell>
-          <cell r="E37">
-            <v>2.2599999999999998</v>
-          </cell>
-          <cell r="F37">
-            <v>6</v>
-          </cell>
-          <cell r="G37">
-            <v>0.4</v>
-          </cell>
-          <cell r="M37">
-            <v>8</v>
-          </cell>
-          <cell r="N37">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>2.2879999999999994</v>
-          </cell>
-          <cell r="D38">
-            <v>2.3239999999999994</v>
-          </cell>
-          <cell r="E38">
-            <v>2.3059999999999992</v>
-          </cell>
-          <cell r="F38">
-            <v>1</v>
-          </cell>
-          <cell r="G38">
-            <v>6.6666666666666666E-2</v>
-          </cell>
-          <cell r="M38">
-            <v>2</v>
-          </cell>
-          <cell r="N38">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39">
-            <v>2.3339999999999992</v>
-          </cell>
-          <cell r="D39">
-            <v>2.3699999999999992</v>
-          </cell>
-          <cell r="E39">
-            <v>2.3519999999999994</v>
-          </cell>
-          <cell r="F39">
-            <v>1</v>
-          </cell>
-          <cell r="G39">
-            <v>6.6666666666666666E-2</v>
-          </cell>
-          <cell r="M39">
-            <v>1</v>
-          </cell>
-          <cell r="N39">
-            <v>14</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="F123" t="str">
-            <v xml:space="preserve">Frecuencia Absoluta </v>
-          </cell>
-          <cell r="G123" t="str">
-            <v xml:space="preserve">Frecuencia Relativa </v>
-          </cell>
-          <cell r="M123" t="str">
-            <v xml:space="preserve">Mayor que </v>
-          </cell>
-          <cell r="N123" t="str">
-            <v xml:space="preserve">Menor que </v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="C124">
-            <v>2.25</v>
-          </cell>
-          <cell r="D124">
-            <v>2.3420000000000001</v>
-          </cell>
-          <cell r="E124">
-            <v>2.2960000000000003</v>
-          </cell>
-          <cell r="F124">
-            <v>8</v>
-          </cell>
-          <cell r="G124">
-            <v>0.53333333333333333</v>
-          </cell>
-          <cell r="M124">
-            <v>15</v>
-          </cell>
-          <cell r="N124">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="C125">
-            <v>2.3519999999999999</v>
-          </cell>
-          <cell r="D125">
-            <v>2.444</v>
-          </cell>
-          <cell r="E125">
-            <v>2.3979999999999997</v>
-          </cell>
-          <cell r="F125">
-            <v>3</v>
-          </cell>
-          <cell r="G125">
-            <v>0.2</v>
-          </cell>
-          <cell r="M125">
-            <v>7</v>
-          </cell>
-          <cell r="N125">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="C126">
-            <v>2.4539999999999997</v>
-          </cell>
-          <cell r="D126">
-            <v>2.5459999999999998</v>
-          </cell>
-          <cell r="E126">
-            <v>2.5</v>
-          </cell>
-          <cell r="F126">
-            <v>2</v>
-          </cell>
-          <cell r="G126">
-            <v>0.13333333333333333</v>
-          </cell>
-          <cell r="M126">
-            <v>4</v>
-          </cell>
-          <cell r="N126">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="C127">
-            <v>2.5559999999999996</v>
-          </cell>
-          <cell r="D127">
-            <v>2.6479999999999997</v>
-          </cell>
-          <cell r="E127">
-            <v>2.6019999999999994</v>
-          </cell>
-          <cell r="F127">
-            <v>1</v>
-          </cell>
-          <cell r="G127">
-            <v>6.6666666666666666E-2</v>
-          </cell>
-          <cell r="M127">
-            <v>2</v>
-          </cell>
-          <cell r="N127">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="C128">
-            <v>2.6579999999999995</v>
-          </cell>
-          <cell r="D128">
-            <v>2.7499999999999996</v>
-          </cell>
-          <cell r="E128">
-            <v>2.7039999999999997</v>
-          </cell>
-          <cell r="F128">
-            <v>1</v>
-          </cell>
-          <cell r="G128">
-            <v>6.6666666666666666E-2</v>
-          </cell>
-          <cell r="M128">
-            <v>1</v>
-          </cell>
-          <cell r="N128">
-            <v>14</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -6221,8 +5731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F52C3B0-17F1-E247-8681-E743B3124AF4}">
   <dimension ref="B4:U84"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="U33" sqref="U33"/>
+    <sheetView topLeftCell="A54" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6235,17 +5745,17 @@
   </cols>
   <sheetData>
     <row r="4" spans="12:16">
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
     </row>
     <row r="6" spans="12:16">
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O6" s="34" t="s">
+      <c r="O6" s="29" t="s">
         <v>2</v>
       </c>
     </row>
@@ -6256,7 +5766,7 @@
       <c r="M7">
         <v>2.15</v>
       </c>
-      <c r="O7" s="35">
+      <c r="O7" s="30">
         <v>2.25</v>
       </c>
       <c r="P7">
@@ -6270,7 +5780,7 @@
       <c r="M8">
         <v>2.1800000000000002</v>
       </c>
-      <c r="O8" s="35">
+      <c r="O8" s="30">
         <v>2.27</v>
       </c>
       <c r="P8">
@@ -6284,7 +5794,7 @@
       <c r="M9">
         <v>2.19</v>
       </c>
-      <c r="O9" s="35">
+      <c r="O9" s="30">
         <v>2.27</v>
       </c>
       <c r="P9">
@@ -6298,7 +5808,7 @@
       <c r="M10">
         <v>2.19</v>
       </c>
-      <c r="O10" s="35">
+      <c r="O10" s="30">
         <v>2.27</v>
       </c>
       <c r="P10">
@@ -6312,7 +5822,7 @@
       <c r="M11">
         <v>2.19</v>
       </c>
-      <c r="O11" s="35">
+      <c r="O11" s="30">
         <v>2.27</v>
       </c>
       <c r="P11">
@@ -6326,7 +5836,7 @@
       <c r="M12">
         <v>2.19</v>
       </c>
-      <c r="O12" s="35">
+      <c r="O12" s="30">
         <v>2.27</v>
       </c>
       <c r="P12">
@@ -6340,7 +5850,7 @@
       <c r="M13">
         <v>2.21</v>
       </c>
-      <c r="O13" s="35">
+      <c r="O13" s="30">
         <v>2.27</v>
       </c>
       <c r="P13">
@@ -6354,7 +5864,7 @@
       <c r="M14">
         <v>2.27</v>
       </c>
-      <c r="O14" s="35">
+      <c r="O14" s="30">
         <v>2.27</v>
       </c>
       <c r="P14">
@@ -6368,7 +5878,7 @@
       <c r="M15">
         <v>2.27</v>
       </c>
-      <c r="O15" s="35">
+      <c r="O15" s="30">
         <v>2.36</v>
       </c>
       <c r="P15">
@@ -6382,7 +5892,7 @@
       <c r="M16">
         <v>2.27</v>
       </c>
-      <c r="O16" s="36">
+      <c r="O16" s="31">
         <v>2.4</v>
       </c>
       <c r="P16">
@@ -6396,7 +5906,7 @@
       <c r="M17">
         <v>2.27</v>
       </c>
-      <c r="O17" s="36">
+      <c r="O17" s="31">
         <v>2.4</v>
       </c>
       <c r="P17">
@@ -6410,7 +5920,7 @@
       <c r="M18">
         <v>2.27</v>
       </c>
-      <c r="O18" s="35">
+      <c r="O18" s="30">
         <v>2.4900000000000002</v>
       </c>
       <c r="P18">
@@ -6424,7 +5934,7 @@
       <c r="M19">
         <v>2.27</v>
       </c>
-      <c r="O19" s="36">
+      <c r="O19" s="31">
         <v>2.5</v>
       </c>
       <c r="P19">
@@ -6435,10 +5945,10 @@
       <c r="L20">
         <v>1</v>
       </c>
-      <c r="M20" s="3">
+      <c r="M20" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="O20" s="35">
+      <c r="O20" s="30">
         <v>2.56</v>
       </c>
       <c r="P20">
@@ -6452,7 +5962,7 @@
       <c r="M21">
         <v>2.33</v>
       </c>
-      <c r="O21" s="35">
+      <c r="O21" s="30">
         <v>2.71</v>
       </c>
       <c r="P21">
@@ -6460,25 +5970,25 @@
       </c>
     </row>
     <row r="23" spans="2:16">
-      <c r="D23" s="4"/>
+      <c r="D23" s="3"/>
     </row>
     <row r="25" spans="2:16" ht="21">
-      <c r="B25" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
+      <c r="B25" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
     </row>
     <row r="27" spans="2:16">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C27">
@@ -6487,10 +5997,10 @@
       </c>
     </row>
     <row r="28" spans="2:16">
-      <c r="B28" s="2"/>
+      <c r="B28" s="1"/>
     </row>
     <row r="29" spans="2:16">
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C29">
@@ -6499,7 +6009,7 @@
       </c>
     </row>
     <row r="30" spans="2:16">
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C30">
@@ -6508,7 +6018,7 @@
       </c>
     </row>
     <row r="31" spans="2:16">
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D31">
@@ -6517,55 +6027,50 @@
       </c>
     </row>
     <row r="32" spans="2:16">
-      <c r="B32" s="2"/>
+      <c r="B32" s="1"/>
     </row>
     <row r="33" spans="2:20">
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="35" spans="2:20" ht="51">
+      <c r="B35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D33">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="35" spans="2:20" ht="51">
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="E35" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="F35" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="G35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="H35" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="I35" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I35" s="7" t="s">
+      <c r="J35" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J35" s="7" t="s">
+      <c r="K35" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K35" s="7" t="s">
+      <c r="L35" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L35" s="7" t="s">
+      <c r="M35" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M35" s="7" t="s">
+      <c r="N35" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="N35" s="7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="36" spans="2:20">
@@ -6587,7 +6092,7 @@
       <c r="F36">
         <v>8</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="7">
         <f>+F36/$F$41</f>
         <v>0.53333333333333333</v>
       </c>
@@ -6595,7 +6100,7 @@
         <f>+F36</f>
         <v>8</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I36" s="8">
         <f>+H36/$F$41</f>
         <v>0.53333333333333333</v>
       </c>
@@ -6605,11 +6110,11 @@
       </c>
       <c r="K36">
         <f>+(E36-$C$46)^2*F36</f>
-        <v>7.2504319999999581E-2</v>
+        <v>5.8984675555555983E-2</v>
       </c>
       <c r="L36">
         <f>+ABS(E36-$C$46)*F36</f>
-        <v>0.76159999999999783</v>
+        <v>0.68693333333333584</v>
       </c>
       <c r="M36">
         <v>15</v>
@@ -6624,20 +6129,20 @@
       </c>
       <c r="C37">
         <f>+D36+$D$33</f>
-        <v>2.3519999999999999</v>
+        <v>2.3420000000000001</v>
       </c>
       <c r="D37">
         <f>+C37+$D$31</f>
-        <v>2.444</v>
+        <v>2.4340000000000002</v>
       </c>
       <c r="E37">
         <f t="shared" ref="E37:E40" si="0">+AVERAGE(C37:D37)</f>
-        <v>2.3979999999999997</v>
+        <v>2.3879999999999999</v>
       </c>
       <c r="F37">
         <v>3</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="7">
         <f t="shared" ref="G37:G40" si="1">+F37/$F$41</f>
         <v>0.2</v>
       </c>
@@ -6645,21 +6150,21 @@
         <f>+H36+F37</f>
         <v>11</v>
       </c>
-      <c r="I37" s="10">
+      <c r="I37" s="8">
         <f t="shared" ref="I37:I40" si="2">+H37/$F$41</f>
         <v>0.73333333333333328</v>
       </c>
       <c r="J37">
         <f t="shared" ref="J37:J40" si="3">+E37*F37</f>
-        <v>7.1939999999999991</v>
+        <v>7.1639999999999997</v>
       </c>
       <c r="K37">
         <f t="shared" ref="K37:K40" si="4">+(E37-$C$46)^2*F37</f>
-        <v>1.3871999999998759E-4</v>
+        <v>1.1285333333330848E-4</v>
       </c>
       <c r="L37">
         <f t="shared" ref="L37:L40" si="5">+ABS(E37-$C$46)*F37</f>
-        <v>2.0399999999999086E-2</v>
+        <v>1.8399999999997974E-2</v>
       </c>
       <c r="M37">
         <f>+M36-F36</f>
@@ -6676,20 +6181,20 @@
       </c>
       <c r="C38">
         <f t="shared" ref="C38:C40" si="6">+D37+$D$33</f>
-        <v>2.4539999999999997</v>
+        <v>2.4340000000000002</v>
       </c>
       <c r="D38">
         <f t="shared" ref="D38:D40" si="7">+C38+$D$31</f>
-        <v>2.5459999999999998</v>
+        <v>2.5260000000000002</v>
       </c>
       <c r="E38">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>2.4800000000000004</v>
       </c>
       <c r="F38">
         <v>2</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="7">
         <f t="shared" si="1"/>
         <v>0.13333333333333333</v>
       </c>
@@ -6697,21 +6202,21 @@
         <f t="shared" ref="H38:H40" si="8">+H37+F38</f>
         <v>13</v>
       </c>
-      <c r="I38" s="10">
+      <c r="I38" s="8">
         <f t="shared" si="2"/>
         <v>0.8666666666666667</v>
       </c>
       <c r="J38">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4.9600000000000009</v>
       </c>
       <c r="K38">
         <f t="shared" si="4"/>
-        <v>2.3674880000000002E-2</v>
+        <v>1.9260302222222164E-2</v>
       </c>
       <c r="L38">
         <f t="shared" si="5"/>
-        <v>0.21760000000000002</v>
+        <v>0.19626666666666637</v>
       </c>
       <c r="M38">
         <f t="shared" ref="M38:M40" si="9">+M37-F37</f>
@@ -6728,20 +6233,20 @@
       </c>
       <c r="C39">
         <f t="shared" si="6"/>
-        <v>2.5559999999999996</v>
+        <v>2.5260000000000002</v>
       </c>
       <c r="D39">
         <f t="shared" si="7"/>
-        <v>2.6479999999999997</v>
+        <v>2.6180000000000003</v>
       </c>
       <c r="E39">
         <f t="shared" si="0"/>
-        <v>2.6019999999999994</v>
+        <v>2.5720000000000001</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="7">
         <f t="shared" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
@@ -6749,21 +6254,21 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="I39" s="10">
+      <c r="I39" s="8">
         <f t="shared" si="2"/>
         <v>0.93333333333333335</v>
       </c>
       <c r="J39">
         <f t="shared" si="3"/>
-        <v>2.6019999999999994</v>
+        <v>2.5720000000000001</v>
       </c>
       <c r="K39">
         <f t="shared" si="4"/>
-        <v>4.4436639999999764E-2</v>
+        <v>3.6150684444444248E-2</v>
       </c>
       <c r="L39">
         <f t="shared" si="5"/>
-        <v>0.21079999999999943</v>
+        <v>0.19013333333333282</v>
       </c>
       <c r="M39">
         <f t="shared" si="9"/>
@@ -6780,20 +6285,20 @@
       </c>
       <c r="C40">
         <f t="shared" si="6"/>
-        <v>2.6579999999999995</v>
+        <v>2.6180000000000003</v>
       </c>
       <c r="D40">
         <f t="shared" si="7"/>
-        <v>2.7499999999999996</v>
+        <v>2.7100000000000004</v>
       </c>
       <c r="E40">
         <f t="shared" si="0"/>
-        <v>2.7039999999999997</v>
+        <v>2.6640000000000006</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G40" s="7">
         <f t="shared" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
@@ -6801,21 +6306,21 @@
         <f t="shared" si="8"/>
         <v>15</v>
       </c>
-      <c r="I40" s="10">
+      <c r="I40" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J40">
         <f t="shared" si="3"/>
-        <v>2.7039999999999997</v>
+        <v>2.6640000000000006</v>
       </c>
       <c r="K40">
         <f t="shared" si="4"/>
-        <v>9.7843839999999835E-2</v>
+        <v>7.9599217777777787E-2</v>
       </c>
       <c r="L40">
         <f t="shared" si="5"/>
-        <v>0.31279999999999974</v>
+        <v>0.28213333333333335</v>
       </c>
       <c r="M40">
         <f t="shared" si="9"/>
@@ -6831,288 +6336,288 @@
         <f>+SUM(F36:F40)</f>
         <v>15</v>
       </c>
-      <c r="G41" s="11">
+      <c r="G41" s="9">
         <f>+SUM(G36:G40)</f>
         <v>1</v>
       </c>
       <c r="J41">
         <f>SUM(J36:J40)</f>
-        <v>35.868000000000002</v>
+        <v>35.728000000000009</v>
       </c>
       <c r="K41">
         <f t="shared" ref="K41:L41" si="11">SUM(K36:K40)</f>
-        <v>0.23859839999999916</v>
+        <v>0.19410773333333348</v>
       </c>
       <c r="L41">
         <f t="shared" si="11"/>
-        <v>1.5231999999999961</v>
+        <v>1.3738666666666663</v>
       </c>
     </row>
     <row r="44" spans="2:20">
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="F44" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="F44" t="s">
+    </row>
+    <row r="46" spans="2:20">
+      <c r="B46" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="46" spans="2:20">
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="10">
+        <f>+J41/F41</f>
+        <v>2.3818666666666672</v>
+      </c>
+      <c r="F46" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="13">
-        <f>+J41/F41</f>
-        <v>2.3912</v>
-      </c>
-      <c r="F46" s="14" t="s">
+      <c r="G46" s="37"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G46" s="14"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="14" t="s">
+      <c r="J46" s="37"/>
+      <c r="M46" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="J46" s="14"/>
-      <c r="M46" s="15" t="s">
+      <c r="N46" s="38"/>
+      <c r="P46" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="N46" s="15"/>
-      <c r="P46" s="1" t="s">
+      <c r="Q46" s="34"/>
+      <c r="R46" s="34"/>
+      <c r="S46" s="34"/>
+      <c r="T46" s="34"/>
+    </row>
+    <row r="47" spans="2:20">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="2:20">
+      <c r="B48" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
-    </row>
-    <row r="47" spans="2:20">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="2:20">
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="10">
+        <f>+C52+(((C50-C54)/C53)*C55)</f>
+        <v>2.2730000000000001</v>
+      </c>
+      <c r="F48" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="13">
-        <f>+C52+(((C50-C54)/C53)*C55)</f>
-        <v>2.2929999999999997</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G48" s="16">
+      <c r="G48" s="11">
         <f>+G50+((G49-G52)/G51)*G53</f>
         <v>2.2931249999999999</v>
       </c>
-      <c r="I48" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="J48" s="18">
+      <c r="I48" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J48" s="13">
         <f>+J50+((J49-J52)/J51)*J53</f>
         <v>2.2586249999999999</v>
       </c>
-      <c r="M48" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="N48" s="19">
+      <c r="M48" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N48" s="14">
         <f>+N50+((N49-N52)/N51)*N53</f>
         <v>2.3362500000000002</v>
       </c>
-      <c r="P48" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q48" s="21">
+      <c r="P48" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q48" s="16">
         <f>SQRT(K41/14)</f>
-        <v>0.1305478565781254</v>
+        <v>0.11774904710968197</v>
       </c>
     </row>
     <row r="49" spans="2:17">
       <c r="B49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C49">
         <f>+F41</f>
         <v>15</v>
       </c>
       <c r="F49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G49">
         <f>+(1*F41)/4</f>
         <v>3.75</v>
       </c>
       <c r="I49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J49">
         <f>+(15*5)/100</f>
         <v>0.75</v>
       </c>
       <c r="M49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N49">
         <f>+(5*F41)/10</f>
         <v>7.5</v>
       </c>
-      <c r="P49" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q49" s="21">
+      <c r="P49" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q49" s="16">
         <f>SQRT(K41/15)</f>
-        <v>0.12612121153874134</v>
+        <v>0.11375638687808068</v>
       </c>
     </row>
     <row r="50" spans="2:17">
       <c r="B50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C50">
         <f>+C49/2</f>
         <v>7.5</v>
       </c>
       <c r="F50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G50">
         <f>+C36</f>
         <v>2.25</v>
       </c>
       <c r="I50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J50">
         <f>+C36</f>
         <v>2.25</v>
       </c>
       <c r="M50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N50">
         <f>+C36</f>
         <v>2.25</v>
       </c>
-      <c r="P50" s="20" t="s">
+      <c r="P50" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q50" s="17">
+        <f>Q48^2</f>
+        <v>1.3864838095238103E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" ht="34">
+      <c r="B51" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="Q50" s="22">
-        <f>Q48^2</f>
-        <v>1.7042742857142797E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="2:17" ht="34">
-      <c r="B51" s="23" t="s">
-        <v>41</v>
       </c>
       <c r="C51">
         <f>+B38</f>
         <v>3</v>
       </c>
       <c r="F51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G51">
         <f>+F36</f>
         <v>8</v>
       </c>
       <c r="I51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J51">
         <f>+F36</f>
         <v>8</v>
       </c>
       <c r="M51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N51">
         <f>+F36</f>
         <v>8</v>
       </c>
-      <c r="P51" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q51" s="22">
+      <c r="P51" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q51" s="17">
         <f>Q49^2</f>
-        <v>1.5906559999999941E-2</v>
+        <v>1.2940515555555566E-2</v>
       </c>
     </row>
     <row r="52" spans="2:17">
       <c r="B52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C52">
         <f>+C38</f>
-        <v>2.4539999999999997</v>
+        <v>2.4340000000000002</v>
       </c>
       <c r="F52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J52">
         <v>0</v>
       </c>
       <c r="M52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N52">
         <v>0</v>
       </c>
-      <c r="P52" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q52" s="24">
+      <c r="P52" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q52" s="19">
         <f>L41/F41</f>
-        <v>0.10154666666666641</v>
+        <v>9.1591111111111095E-2</v>
       </c>
     </row>
     <row r="53" spans="2:17">
       <c r="B53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C53">
         <f>+F38</f>
         <v>2</v>
       </c>
       <c r="F53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G53">
         <f>+D31</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="I53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J53">
         <f>+D31</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="M53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N53">
         <f>+D31</f>
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="P53" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q53" s="25">
+      <c r="P53" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q53" s="20">
         <f>Q48/C46</f>
-        <v>5.4595122356191621E-2</v>
+        <v>4.9435616509326832E-2</v>
       </c>
     </row>
     <row r="54" spans="2:17">
       <c r="B54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C54">
         <f>+H37</f>
@@ -7121,51 +6626,51 @@
     </row>
     <row r="55" spans="2:17">
       <c r="B55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55">
         <f>+D31</f>
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="F55" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="G55" s="16">
+      <c r="F55" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G55" s="11">
         <f>+G57+((G56-G59)/G58)*G60</f>
         <v>2.3362500000000002</v>
       </c>
-      <c r="I55" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="J55" s="17">
+      <c r="I55" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J55" s="12">
         <f>+J57+((J56-J59)/J58)*J60</f>
         <v>2.3362500000000002</v>
       </c>
-      <c r="M55" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="N55" s="19">
+      <c r="M55" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="N55" s="14">
         <f>+N57+((N56-N59)/N58)*N60</f>
-        <v>2.7499999999999996</v>
+        <v>2.7100000000000004</v>
       </c>
     </row>
     <row r="56" spans="2:17">
       <c r="F56" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G56">
         <f>+(2*15)/4</f>
         <v>7.5</v>
       </c>
       <c r="I56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J56">
         <f>+(50*F41)/100</f>
         <v>7.5</v>
       </c>
       <c r="M56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N56">
         <f>+(10*F41)/10</f>
@@ -7173,59 +6678,59 @@
       </c>
     </row>
     <row r="57" spans="2:17">
-      <c r="B57" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57" s="13">
+      <c r="B57" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" s="10">
         <f>+C59+((C60-C62)/(2*C60-C61-C62))*C63</f>
         <v>2.3036666666666665</v>
       </c>
       <c r="F57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G57">
         <f>+C36</f>
         <v>2.25</v>
       </c>
       <c r="I57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J57">
         <f>+C36</f>
         <v>2.25</v>
       </c>
       <c r="M57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N57">
         <f>+C40</f>
-        <v>2.6579999999999995</v>
+        <v>2.6180000000000003</v>
       </c>
     </row>
     <row r="58" spans="2:17">
       <c r="B58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C58">
         <f>+B36</f>
         <v>1</v>
       </c>
       <c r="F58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G58">
         <f>+F36</f>
         <v>8</v>
       </c>
       <c r="I58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J58">
         <f>+F36</f>
         <v>8</v>
       </c>
       <c r="M58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N58">
         <f>+F40</f>
@@ -7234,26 +6739,26 @@
     </row>
     <row r="59" spans="2:17">
       <c r="B59" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C59">
         <f>+C36</f>
         <v>2.25</v>
       </c>
       <c r="F59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J59">
         <v>0</v>
       </c>
       <c r="M59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N59">
         <f>+H39</f>
@@ -7262,28 +6767,28 @@
     </row>
     <row r="60" spans="2:17">
       <c r="B60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C60">
         <f>+F36</f>
         <v>8</v>
       </c>
       <c r="F60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G60">
         <f>+D31</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="I60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J60">
         <f>+D31</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="M60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N60">
         <f>+D31</f>
@@ -7292,7 +6797,7 @@
     </row>
     <row r="61" spans="2:17">
       <c r="B61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C61">
         <f>+F37</f>
@@ -7301,44 +6806,44 @@
     </row>
     <row r="62" spans="2:17">
       <c r="B62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C62">
         <f>+F40</f>
         <v>1</v>
       </c>
-      <c r="F62" s="16" t="s">
+      <c r="F62" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G62" s="11">
+        <f>+G64+((G63-G66)/G65)*G67</f>
+        <v>2.4455</v>
+      </c>
+      <c r="I62" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G62" s="16">
-        <f>+G64+((G63-G66)/G65)*G67</f>
-        <v>2.4654999999999996</v>
-      </c>
-      <c r="I62" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J62" s="17">
+      <c r="J62" s="12">
         <f>+J64+((J63-J66)/J65)*J67</f>
-        <v>2.6809999999999996</v>
+        <v>2.6410000000000005</v>
       </c>
     </row>
     <row r="63" spans="2:17">
       <c r="B63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C63">
         <f>+D31</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="F63" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G63">
         <f>+(3*15)/4</f>
         <v>11.25</v>
       </c>
       <c r="I63" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J63">
         <f>+(95*F41)/100</f>
@@ -7347,30 +6852,30 @@
     </row>
     <row r="64" spans="2:17">
       <c r="F64" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G64">
         <f>+C38</f>
-        <v>2.4539999999999997</v>
+        <v>2.4340000000000002</v>
       </c>
       <c r="I64" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J64">
         <f>+C40</f>
-        <v>2.6579999999999995</v>
+        <v>2.6180000000000003</v>
       </c>
     </row>
     <row r="65" spans="6:21">
       <c r="F65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G65">
         <f>+F38</f>
         <v>2</v>
       </c>
       <c r="I65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J65">
         <f>+F40</f>
@@ -7379,14 +6884,14 @@
     </row>
     <row r="66" spans="6:21">
       <c r="F66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G66">
         <f>+H37</f>
         <v>11</v>
       </c>
       <c r="I66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J66">
         <f>+H39</f>
@@ -7395,14 +6900,14 @@
     </row>
     <row r="67" spans="6:21">
       <c r="F67" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G67">
         <f>+D31</f>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="I67" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J67">
         <f>+D31</f>
@@ -7410,56 +6915,56 @@
       </c>
     </row>
     <row r="71" spans="6:21">
-      <c r="O71" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P71" s="1"/>
-      <c r="Q71" s="1"/>
-      <c r="R71" s="1"/>
+      <c r="O71" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="P71" s="34"/>
+      <c r="Q71" s="34"/>
+      <c r="R71" s="34"/>
     </row>
     <row r="73" spans="6:21">
-      <c r="O73" s="27"/>
-      <c r="Q73" s="28"/>
-      <c r="R73" s="29"/>
-      <c r="S73" s="29"/>
-      <c r="U73" s="30"/>
+      <c r="O73" s="22"/>
+      <c r="Q73" s="23"/>
+      <c r="R73" s="24"/>
+      <c r="S73" s="24"/>
+      <c r="U73" s="25"/>
     </row>
     <row r="74" spans="6:21">
-      <c r="O74" s="31"/>
-      <c r="P74" s="32"/>
-      <c r="Q74" s="27"/>
-      <c r="R74" s="30"/>
-      <c r="S74" s="30"/>
-      <c r="T74" s="31"/>
-      <c r="U74" s="32"/>
+      <c r="O74" s="26"/>
+      <c r="P74" s="27"/>
+      <c r="Q74" s="22"/>
+      <c r="R74" s="25"/>
+      <c r="S74" s="25"/>
+      <c r="T74" s="26"/>
+      <c r="U74" s="27"/>
     </row>
     <row r="75" spans="6:21">
-      <c r="O75" s="27"/>
-      <c r="Q75" s="27"/>
-      <c r="R75" s="30"/>
-      <c r="S75" s="30"/>
-      <c r="U75" s="30"/>
+      <c r="O75" s="22"/>
+      <c r="Q75" s="22"/>
+      <c r="R75" s="25"/>
+      <c r="S75" s="25"/>
+      <c r="U75" s="25"/>
     </row>
     <row r="76" spans="6:21">
-      <c r="O76" s="27"/>
-      <c r="Q76" s="31"/>
-      <c r="R76" s="32"/>
-      <c r="S76" s="32"/>
-      <c r="U76" s="30"/>
+      <c r="O76" s="22"/>
+      <c r="Q76" s="26"/>
+      <c r="R76" s="27"/>
+      <c r="S76" s="27"/>
+      <c r="U76" s="25"/>
     </row>
     <row r="77" spans="6:21">
-      <c r="O77" s="31"/>
-      <c r="P77" s="33"/>
-      <c r="Q77" s="33"/>
-      <c r="R77" s="33"/>
-      <c r="S77" s="33"/>
-      <c r="T77" s="33"/>
-      <c r="U77" s="32"/>
+      <c r="O77" s="26"/>
+      <c r="P77" s="28"/>
+      <c r="Q77" s="28"/>
+      <c r="R77" s="28"/>
+      <c r="S77" s="28"/>
+      <c r="T77" s="28"/>
+      <c r="U77" s="27"/>
     </row>
     <row r="78" spans="6:21">
       <c r="O78">
         <f>+P83</f>
-        <v>2.0345625000000003</v>
+        <v>2.0645624999999996</v>
       </c>
       <c r="Q78">
         <f>+G48</f>
@@ -7467,57 +6972,58 @@
       </c>
       <c r="R78">
         <f>+C46</f>
-        <v>2.3912</v>
+        <v>2.3818666666666672</v>
       </c>
       <c r="S78">
         <f>+G62</f>
-        <v>2.4654999999999996</v>
+        <v>2.4455</v>
       </c>
       <c r="U78">
         <f>+P84</f>
-        <v>2.7240624999999992</v>
+        <v>2.6740625000000002</v>
       </c>
     </row>
     <row r="79" spans="6:21">
-      <c r="Q79" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R79" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="S79" s="26" t="s">
-        <v>60</v>
+      <c r="Q79" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R79" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S79" s="21" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="15:17">
       <c r="O81" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q81">
         <f>+G62-G48</f>
-        <v>0.17237499999999972</v>
+        <v>0.15237500000000015</v>
       </c>
     </row>
     <row r="83" spans="15:17">
       <c r="O83" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P83">
         <f>+Q78-1.5*(Q81)</f>
-        <v>2.0345625000000003</v>
+        <v>2.0645624999999996</v>
       </c>
     </row>
     <row r="84" spans="15:17">
       <c r="O84" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P84">
         <f>+S78+1.5*(Q81)</f>
-        <v>2.7240624999999992</v>
+        <v>2.6740625000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="M4:O4"/>
     <mergeCell ref="O71:R71"/>
     <mergeCell ref="B25:L25"/>
     <mergeCell ref="B44:D44"/>
@@ -7525,7 +7031,6 @@
     <mergeCell ref="I46:J46"/>
     <mergeCell ref="M46:N46"/>
     <mergeCell ref="P46:T46"/>
-    <mergeCell ref="M4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7537,7 +7042,7 @@
   <dimension ref="B2:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7549,120 +7054,120 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="37" t="s">
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="33">
+        <v>1360</v>
+      </c>
+      <c r="C4" s="2">
+        <v>278.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="33">
+        <v>1940</v>
+      </c>
+      <c r="C5" s="2">
+        <v>375.7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="33">
+        <v>1750</v>
+      </c>
+      <c r="C6" s="2">
+        <v>339.5</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4" s="38">
-        <v>1360</v>
-      </c>
-      <c r="C4" s="3">
-        <v>278.5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="38">
-        <v>1940</v>
-      </c>
-      <c r="C5" s="3">
-        <v>375.7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="38">
-        <v>1750</v>
-      </c>
-      <c r="C6" s="3">
-        <v>339.5</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <f>+CORREL(B4:B15,C4:C15)</f>
         <v>0.92414002878207713</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="38">
+      <c r="B7" s="33">
         <v>1550</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>329.8</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="1">
         <f>+_xlfn.COVARIANCE.S(B4:B15,C4:C15)</f>
         <v>15545.196969696968</v>
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="38">
+      <c r="B8" s="33">
         <v>1790</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>295.60000000000002</v>
       </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="38">
+      <c r="B9" s="33">
         <v>1750</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>310.3</v>
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="38">
+      <c r="B10" s="33">
         <v>2230</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>460.5</v>
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="38">
+      <c r="B11" s="33">
         <v>1600</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>305.2</v>
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="38">
+      <c r="B12" s="33">
         <v>1450</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>288.60000000000002</v>
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="38">
+      <c r="B13" s="33">
         <v>1870</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>365.7</v>
       </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="38">
+      <c r="B14" s="33">
         <v>2210</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>425.3</v>
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="38">
+      <c r="B15" s="33">
         <v>1480</v>
       </c>
-      <c r="C15" s="38">
+      <c r="C15" s="33">
         <v>268.8</v>
       </c>
     </row>

</xml_diff>